<commit_message>
Added Gompertz calculation for uZM
</commit_message>
<xml_diff>
--- a/Inijalni parametri GM Modela.xlsx
+++ b/Inijalni parametri GM Modela.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>beta_1</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>ZM</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,6 +407,17 @@
         <v>3.1449999999999999E-2</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2.7550000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>3.1449999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>